<commit_message>
2m x 1024 BIOS set
</commit_message>
<xml_diff>
--- a/ariel_results/per_function_timing/tree_timings_2m_x_1024.xlsx
+++ b/ariel_results/per_function_timing/tree_timings_2m_x_1024.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,885 +434,825 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>tree</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Selecting Bootstrapped Samples</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Initialization of FindBestCondOblique</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>SampleProjection</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>ApplyProjection</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Bucket Allocation &amp; Initialization=0</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Filling &amp; Finalizing the Buckets</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>SortFeature</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>ScanSplits</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Post-processing after Training all Trees</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>EvaluateProjection</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>FillExampleBucketSet (next 3 calls)</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0.242029</v>
       </c>
       <c r="C2" t="n">
-        <v>0.11561</v>
+        <v>0.0215653</v>
       </c>
       <c r="D2" t="n">
-        <v>0.00528134</v>
+        <v>2.3317e-05</v>
       </c>
       <c r="E2" t="n">
-        <v>4.996e-06</v>
+        <v>0.032588</v>
       </c>
       <c r="F2" t="n">
-        <v>0.00755692</v>
+        <v>0.0156106</v>
       </c>
       <c r="G2" t="n">
-        <v>0.00410217</v>
+        <v>5.9e-08</v>
       </c>
       <c r="H2" t="n">
-        <v>2e-08</v>
+        <v>0.556986</v>
       </c>
       <c r="I2" t="n">
-        <v>0.116655</v>
+        <v>0.0451566</v>
       </c>
       <c r="J2" t="n">
-        <v>0.020633</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>0.625959</v>
       </c>
       <c r="L2" t="n">
-        <v>0.143795</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0.122445</v>
+        <v>0.578371</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>0.558399</v>
       </c>
       <c r="C3" t="n">
-        <v>0.115112</v>
+        <v>0.0213369</v>
       </c>
       <c r="D3" t="n">
-        <v>0.00520424</v>
+        <v>9.659e-06</v>
       </c>
       <c r="E3" t="n">
-        <v>4.026e-06</v>
+        <v>0.0327094</v>
       </c>
       <c r="F3" t="n">
-        <v>0.00759597</v>
+        <v>0.0163864</v>
       </c>
       <c r="G3" t="n">
-        <v>0.00419637</v>
+        <v>6.1e-08</v>
       </c>
       <c r="H3" t="n">
-        <v>1.8e-08</v>
+        <v>0.251032</v>
       </c>
       <c r="I3" t="n">
-        <v>0.118439</v>
+        <v>0.0393636</v>
       </c>
       <c r="J3" t="n">
-        <v>0.0204471</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>0.314867</v>
       </c>
       <c r="L3" t="n">
-        <v>0.145802</v>
-      </c>
-      <c r="M3" t="n">
-        <v>0.124646</v>
+        <v>0.273108</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>0.230608</v>
       </c>
       <c r="C4" t="n">
-        <v>0.112497</v>
+        <v>0.00298671</v>
       </c>
       <c r="D4" t="n">
-        <v>0.00286859</v>
+        <v>4.758e-06</v>
       </c>
       <c r="E4" t="n">
-        <v>3.064e-06</v>
+        <v>0.0104228</v>
       </c>
       <c r="F4" t="n">
-        <v>0.00567357</v>
+        <v>0.0148703</v>
       </c>
       <c r="G4" t="n">
-        <v>0.00407049</v>
+        <v>1.05e-07</v>
       </c>
       <c r="H4" t="n">
-        <v>2e-08</v>
+        <v>0.565041</v>
       </c>
       <c r="I4" t="n">
-        <v>0.117862</v>
+        <v>0.136657</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0201536</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>0.723727</v>
       </c>
       <c r="L4" t="n">
-        <v>0.144495</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.123642</v>
+        <v>0.585778</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
+      <c r="A5" t="n">
+        <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>0.237038</v>
       </c>
       <c r="C5" t="n">
-        <v>0.111622</v>
+        <v>0.0030341</v>
       </c>
       <c r="D5" t="n">
-        <v>0.00259647</v>
+        <v>4.198e-06</v>
       </c>
       <c r="E5" t="n">
-        <v>3.545e-06</v>
+        <v>0.0103909</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0058342</v>
+        <v>0.007933229999999999</v>
       </c>
       <c r="G5" t="n">
-        <v>0.00430767</v>
+        <v>3.8e-08</v>
       </c>
       <c r="H5" t="n">
-        <v>1.9e-08</v>
+        <v>0.557119</v>
       </c>
       <c r="I5" t="n">
-        <v>0.117046</v>
+        <v>0.0461574</v>
       </c>
       <c r="J5" t="n">
-        <v>0.020221</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>0.615267</v>
       </c>
       <c r="L5" t="n">
-        <v>0.143994</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.123059</v>
+        <v>0.567814</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
+      <c r="A6" t="n">
+        <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>0.237913</v>
       </c>
       <c r="C6" t="n">
-        <v>0.112036</v>
+        <v>0.00639337</v>
       </c>
       <c r="D6" t="n">
-        <v>0.00257741</v>
+        <v>1.0251e-05</v>
       </c>
       <c r="E6" t="n">
-        <v>5.215e-06</v>
+        <v>0.0254825</v>
       </c>
       <c r="F6" t="n">
-        <v>0.00587173</v>
+        <v>0.00761433</v>
       </c>
       <c r="G6" t="n">
-        <v>0.00404496</v>
+        <v>3.7e-08</v>
       </c>
       <c r="H6" t="n">
-        <v>1.8e-08</v>
+        <v>0.243906</v>
       </c>
       <c r="I6" t="n">
-        <v>0.117169</v>
+        <v>0.0393458</v>
       </c>
       <c r="J6" t="n">
-        <v>0.0202838</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>0.295867</v>
       </c>
       <c r="L6" t="n">
-        <v>0.143947</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.122968</v>
+        <v>0.254374</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
+      <c r="A7" t="n">
+        <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>6</v>
+        <v>0.237926</v>
       </c>
       <c r="C7" t="n">
-        <v>0.112088</v>
+        <v>0.0030022</v>
       </c>
       <c r="D7" t="n">
-        <v>0.00261553</v>
+        <v>4.134e-06</v>
       </c>
       <c r="E7" t="n">
-        <v>4.718e-06</v>
+        <v>0.0104721</v>
       </c>
       <c r="F7" t="n">
-        <v>0.00583911</v>
+        <v>0.00753389</v>
       </c>
       <c r="G7" t="n">
-        <v>0.00404645</v>
+        <v>2.4e-08</v>
       </c>
       <c r="H7" t="n">
-        <v>1.2e-08</v>
+        <v>0.243578</v>
       </c>
       <c r="I7" t="n">
-        <v>0.118125</v>
+        <v>0.0395325</v>
       </c>
       <c r="J7" t="n">
-        <v>0.0204776</v>
+        <v>0</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>0.294607</v>
       </c>
       <c r="L7" t="n">
-        <v>0.145076</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0.123888</v>
+        <v>0.25384</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
+      <c r="A8" t="n">
+        <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>7</v>
+        <v>0.237385</v>
       </c>
       <c r="C8" t="n">
-        <v>0.112655</v>
+        <v>0.00687301</v>
       </c>
       <c r="D8" t="n">
-        <v>0.00232749</v>
+        <v>9.764e-06</v>
       </c>
       <c r="E8" t="n">
-        <v>3.354e-06</v>
+        <v>0.0255454</v>
       </c>
       <c r="F8" t="n">
-        <v>0.00569904</v>
+        <v>0.0148236</v>
       </c>
       <c r="G8" t="n">
-        <v>0.00403486</v>
+        <v>1.03e-07</v>
       </c>
       <c r="H8" t="n">
-        <v>1.4e-08</v>
+        <v>0.562206</v>
       </c>
       <c r="I8" t="n">
-        <v>0.117025</v>
+        <v>0.0782926</v>
       </c>
       <c r="J8" t="n">
-        <v>0.0201468</v>
+        <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>0.6636030000000001</v>
       </c>
       <c r="L8" t="n">
-        <v>0.143638</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.122773</v>
+        <v>0.582871</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
+      <c r="A9" t="n">
+        <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>8</v>
+        <v>0.236423</v>
       </c>
       <c r="C9" t="n">
-        <v>0.111392</v>
+        <v>0.00296234</v>
       </c>
       <c r="D9" t="n">
-        <v>0.00258175</v>
+        <v>8.410000000000001e-06</v>
       </c>
       <c r="E9" t="n">
-        <v>4.083e-06</v>
+        <v>0.0103868</v>
       </c>
       <c r="F9" t="n">
-        <v>0.00588756</v>
+        <v>0.007917169999999999</v>
       </c>
       <c r="G9" t="n">
-        <v>0.00423685</v>
+        <v>3.7e-08</v>
       </c>
       <c r="H9" t="n">
-        <v>1.9e-08</v>
+        <v>0.242769</v>
       </c>
       <c r="I9" t="n">
-        <v>0.116454</v>
+        <v>0.0395579</v>
       </c>
       <c r="J9" t="n">
-        <v>0.0204747</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>0.294222</v>
       </c>
       <c r="L9" t="n">
-        <v>0.143581</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0.122412</v>
+        <v>0.253439</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
+      <c r="A10" t="n">
+        <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>9</v>
+        <v>0.237244</v>
       </c>
       <c r="C10" t="n">
-        <v>0.11244</v>
+        <v>0.00304514</v>
       </c>
       <c r="D10" t="n">
-        <v>0.00279</v>
+        <v>4.079e-06</v>
       </c>
       <c r="E10" t="n">
-        <v>3.201e-06</v>
+        <v>0.0104228</v>
       </c>
       <c r="F10" t="n">
-        <v>0.00602171</v>
+        <v>0.00801702</v>
       </c>
       <c r="G10" t="n">
-        <v>0.00409339</v>
+        <v>2.6e-08</v>
       </c>
       <c r="H10" t="n">
-        <v>1.39e-07</v>
+        <v>0.243558</v>
       </c>
       <c r="I10" t="n">
-        <v>0.116743</v>
+        <v>0.0394343</v>
       </c>
       <c r="J10" t="n">
-        <v>0.0203769</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>0.295027</v>
       </c>
       <c r="L10" t="n">
-        <v>0.143605</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0.122548</v>
+        <v>0.254359</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
+      <c r="A11" t="n">
+        <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>10</v>
+        <v>0.546742</v>
       </c>
       <c r="C11" t="n">
-        <v>0.112412</v>
+        <v>0.00681116</v>
       </c>
       <c r="D11" t="n">
-        <v>0.00260856</v>
+        <v>1.2816e-05</v>
       </c>
       <c r="E11" t="n">
-        <v>3.248e-06</v>
+        <v>0.0257595</v>
       </c>
       <c r="F11" t="n">
-        <v>0.00606914</v>
+        <v>0.015856</v>
       </c>
       <c r="G11" t="n">
-        <v>0.00413225</v>
+        <v>9.7e-08</v>
       </c>
       <c r="H11" t="n">
-        <v>1.3e-08</v>
+        <v>0.307702</v>
       </c>
       <c r="I11" t="n">
-        <v>0.117469</v>
+        <v>0.0902881</v>
       </c>
       <c r="J11" t="n">
-        <v>0.020143</v>
+        <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>0.421946</v>
       </c>
       <c r="L11" t="n">
-        <v>0.14424</v>
-      </c>
-      <c r="M11" t="n">
-        <v>0.123363</v>
+        <v>0.329233</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
+      <c r="A12" t="n">
+        <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>11</v>
+        <v>0.238879</v>
       </c>
       <c r="C12" t="n">
-        <v>0.113561</v>
+        <v>0.00296705</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0026689</v>
+        <v>4.004e-06</v>
       </c>
       <c r="E12" t="n">
-        <v>3.028e-06</v>
+        <v>0.0104247</v>
       </c>
       <c r="F12" t="n">
-        <v>0.00574827</v>
+        <v>0.00169009</v>
       </c>
       <c r="G12" t="n">
-        <v>0.00119438</v>
+        <v>3.7e-08</v>
       </c>
       <c r="H12" t="n">
-        <v>1.8e-08</v>
+        <v>0.24502</v>
       </c>
       <c r="I12" t="n">
-        <v>0.118093</v>
+        <v>0.0667845</v>
       </c>
       <c r="J12" t="n">
-        <v>0.0204782</v>
+        <v>0</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>0.3175</v>
       </c>
       <c r="L12" t="n">
-        <v>0.142357</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0.121169</v>
+        <v>0.249412</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
+      <c r="A13" t="n">
+        <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>12</v>
+        <v>0.578454</v>
       </c>
       <c r="C13" t="n">
-        <v>0.112032</v>
+        <v>0.00645447</v>
       </c>
       <c r="D13" t="n">
-        <v>0.00256167</v>
+        <v>1.0781e-05</v>
       </c>
       <c r="E13" t="n">
-        <v>2.921e-06</v>
+        <v>0.0254714</v>
       </c>
       <c r="F13" t="n">
-        <v>0.00589387</v>
+        <v>0.00328704</v>
       </c>
       <c r="G13" t="n">
-        <v>0.00119247</v>
+        <v>7.7e-08</v>
       </c>
       <c r="H13" t="n">
-        <v>1.3e-08</v>
+        <v>0.564482</v>
       </c>
       <c r="I13" t="n">
-        <v>0.116917</v>
+        <v>0.0571513</v>
       </c>
       <c r="J13" t="n">
-        <v>0.020238</v>
+        <v>0</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>0.633122</v>
       </c>
       <c r="L13" t="n">
-        <v>0.140728</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0.119797</v>
+        <v>0.5735209999999999</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
+      <c r="A14" t="n">
+        <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>13</v>
+        <v>0.2372</v>
       </c>
       <c r="C14" t="n">
-        <v>0.111796</v>
+        <v>0.00295307</v>
       </c>
       <c r="D14" t="n">
-        <v>0.00257812</v>
+        <v>3.823e-06</v>
       </c>
       <c r="E14" t="n">
-        <v>2.887e-06</v>
+        <v>0.0103876</v>
       </c>
       <c r="F14" t="n">
-        <v>0.00600134</v>
+        <v>0.00167369</v>
       </c>
       <c r="G14" t="n">
-        <v>0.00119739</v>
+        <v>3.6e-08</v>
       </c>
       <c r="H14" t="n">
-        <v>1.8e-08</v>
+        <v>0.237557</v>
       </c>
       <c r="I14" t="n">
-        <v>0.117345</v>
+        <v>0.0391434</v>
       </c>
       <c r="J14" t="n">
-        <v>0.0202644</v>
+        <v>0</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>0.282343</v>
       </c>
       <c r="L14" t="n">
-        <v>0.14125</v>
-      </c>
-      <c r="M14" t="n">
-        <v>0.120302</v>
+        <v>0.241975</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
+      <c r="A15" t="n">
+        <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>14</v>
+        <v>0.258317</v>
       </c>
       <c r="C15" t="n">
-        <v>0.112077</v>
+        <v>0.00299546</v>
       </c>
       <c r="D15" t="n">
-        <v>0.00255032</v>
+        <v>4.698e-06</v>
       </c>
       <c r="E15" t="n">
-        <v>3.053e-06</v>
+        <v>0.0104069</v>
       </c>
       <c r="F15" t="n">
-        <v>0.00565843</v>
+        <v>0.00170717</v>
       </c>
       <c r="G15" t="n">
-        <v>0.00119364</v>
+        <v>3.7e-08</v>
       </c>
       <c r="H15" t="n">
-        <v>2e-08</v>
+        <v>0.245003</v>
       </c>
       <c r="I15" t="n">
-        <v>0.117728</v>
+        <v>0.101772</v>
       </c>
       <c r="J15" t="n">
-        <v>0.0202095</v>
+        <v>0</v>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>0.35261</v>
       </c>
       <c r="L15" t="n">
-        <v>0.141542</v>
-      </c>
-      <c r="M15" t="n">
-        <v>0.120642</v>
+        <v>0.249568</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
+      <c r="A16" t="n">
+        <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>15</v>
+        <v>0.517726</v>
       </c>
       <c r="C16" t="n">
-        <v>0.110786</v>
+        <v>0.00298766</v>
       </c>
       <c r="D16" t="n">
-        <v>0.00265188</v>
+        <v>5.312e-06</v>
       </c>
       <c r="E16" t="n">
-        <v>3.159e-06</v>
+        <v>0.0104</v>
       </c>
       <c r="F16" t="n">
-        <v>0.00578841</v>
+        <v>0.00168765</v>
       </c>
       <c r="G16" t="n">
-        <v>0.00119234</v>
+        <v>3.6e-08</v>
       </c>
       <c r="H16" t="n">
-        <v>1.3e-08</v>
+        <v>0.244695</v>
       </c>
       <c r="I16" t="n">
-        <v>0.118017</v>
+        <v>0.0393235</v>
       </c>
       <c r="J16" t="n">
-        <v>0.0201914</v>
+        <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>0.289632</v>
       </c>
       <c r="L16" t="n">
-        <v>0.14191</v>
-      </c>
-      <c r="M16" t="n">
-        <v>0.121035</v>
+        <v>0.249084</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
+      <c r="A17" t="n">
+        <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>16</v>
+        <v>0.578913</v>
       </c>
       <c r="C17" t="n">
-        <v>0.112604</v>
+        <v>0.00321551</v>
       </c>
       <c r="D17" t="n">
-        <v>0.00260566</v>
+        <v>5.459e-06</v>
       </c>
       <c r="E17" t="n">
-        <v>3.062e-06</v>
+        <v>0.0104339</v>
       </c>
       <c r="F17" t="n">
-        <v>0.00580703</v>
+        <v>0.00172083</v>
       </c>
       <c r="G17" t="n">
-        <v>0.00119717</v>
+        <v>3.6e-08</v>
       </c>
       <c r="H17" t="n">
-        <v>1.8e-08</v>
+        <v>0.244183</v>
       </c>
       <c r="I17" t="n">
-        <v>0.117224</v>
+        <v>0.0392907</v>
       </c>
       <c r="J17" t="n">
-        <v>0.0202568</v>
+        <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>0.289156</v>
       </c>
       <c r="L17" t="n">
-        <v>0.141169</v>
-      </c>
-      <c r="M17" t="n">
-        <v>0.120186</v>
+        <v>0.248646</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
+      <c r="A18" t="n">
+        <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>17</v>
+        <v>0.226558</v>
       </c>
       <c r="C18" t="n">
-        <v>0.111196</v>
+        <v>0.00293707</v>
       </c>
       <c r="D18" t="n">
-        <v>0.00260775</v>
+        <v>3.076e-06</v>
       </c>
       <c r="E18" t="n">
-        <v>3.325e-06</v>
+        <v>0.0104319</v>
       </c>
       <c r="F18" t="n">
-        <v>0.00589602</v>
+        <v>0.00166165</v>
       </c>
       <c r="G18" t="n">
-        <v>0.00120296</v>
+        <v>2.6e-08</v>
       </c>
       <c r="H18" t="n">
-        <v>9.9e-08</v>
+        <v>0.235189</v>
       </c>
       <c r="I18" t="n">
-        <v>0.117142</v>
+        <v>0.0392393</v>
       </c>
       <c r="J18" t="n">
-        <v>0.0220286</v>
+        <v>0</v>
       </c>
       <c r="K18" t="n">
-        <v>0</v>
+        <v>0.280024</v>
       </c>
       <c r="L18" t="n">
-        <v>0.142784</v>
-      </c>
-      <c r="M18" t="n">
-        <v>0.120055</v>
+        <v>0.239549</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
+      <c r="A19" t="n">
+        <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>18</v>
+        <v>0.230629</v>
       </c>
       <c r="C19" t="n">
-        <v>0.113556</v>
+        <v>0.00680067</v>
       </c>
       <c r="D19" t="n">
-        <v>0.00273699</v>
+        <v>1.2526e-05</v>
       </c>
       <c r="E19" t="n">
-        <v>3.889e-06</v>
+        <v>0.0254089</v>
       </c>
       <c r="F19" t="n">
-        <v>0.00591086</v>
+        <v>0.00336038</v>
       </c>
       <c r="G19" t="n">
-        <v>0.00120032</v>
+        <v>6.1e-08</v>
       </c>
       <c r="H19" t="n">
-        <v>1.9e-08</v>
+        <v>0.565538</v>
       </c>
       <c r="I19" t="n">
-        <v>0.117479</v>
+        <v>0.120725</v>
       </c>
       <c r="J19" t="n">
-        <v>0.0201694</v>
+        <v>0</v>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>0.697801</v>
       </c>
       <c r="L19" t="n">
-        <v>0.141375</v>
-      </c>
-      <c r="M19" t="n">
-        <v>0.120495</v>
+        <v>0.574608</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
+      <c r="A20" t="n">
+        <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>19</v>
+        <v>0.46698</v>
       </c>
       <c r="C20" t="n">
-        <v>0.111961</v>
+        <v>0.00308403</v>
       </c>
       <c r="D20" t="n">
-        <v>0.00264684</v>
+        <v>4.558e-06</v>
       </c>
       <c r="E20" t="n">
-        <v>2.744e-06</v>
+        <v>0.0104002</v>
       </c>
       <c r="F20" t="n">
-        <v>0.00602287</v>
+        <v>0.00166454</v>
       </c>
       <c r="G20" t="n">
-        <v>0.00120038</v>
+        <v>3.8e-08</v>
       </c>
       <c r="H20" t="n">
-        <v>1.3e-08</v>
+        <v>0.552562</v>
       </c>
       <c r="I20" t="n">
-        <v>0.117222</v>
+        <v>0.120466</v>
       </c>
       <c r="J20" t="n">
-        <v>0.0201983</v>
+        <v>0</v>
       </c>
       <c r="K20" t="n">
-        <v>0</v>
+        <v>0.678681</v>
       </c>
       <c r="L20" t="n">
-        <v>0.14106</v>
-      </c>
-      <c r="M20" t="n">
-        <v>0.120162</v>
+        <v>0.556949</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
+      <c r="A21" t="n">
+        <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>20</v>
+        <v>0.574527</v>
       </c>
       <c r="C21" t="n">
-        <v>0.111973</v>
+        <v>0.00633003</v>
       </c>
       <c r="D21" t="n">
-        <v>0.00258633</v>
+        <v>1.1117e-05</v>
       </c>
       <c r="E21" t="n">
-        <v>2.316e-06</v>
+        <v>0.0254525</v>
       </c>
       <c r="F21" t="n">
-        <v>0.00575942</v>
+        <v>0.00325047</v>
       </c>
       <c r="G21" t="n">
-        <v>0.00118066</v>
+        <v>7.7e-08</v>
       </c>
       <c r="H21" t="n">
-        <v>1.2e-08</v>
+        <v>0.5649380000000001</v>
       </c>
       <c r="I21" t="n">
-        <v>0.117406</v>
+        <v>0.120566</v>
       </c>
       <c r="J21" t="n">
-        <v>0.0203586</v>
+        <v>0.000712843</v>
       </c>
       <c r="K21" t="n">
-        <v>0.00774594</v>
+        <v>0.697026</v>
       </c>
       <c r="L21" t="n">
-        <v>0.141428</v>
-      </c>
-      <c r="M21" t="n">
-        <v>0.120379</v>
+        <v>0.573972</v>
       </c>
     </row>
   </sheetData>

</xml_diff>